<commit_message>
Updated file on 22-11-2017 @ 5.35 pm
</commit_message>
<xml_diff>
--- a/Project-Status.xlsx
+++ b/Project-Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Status</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>21/11/2017</t>
+  </si>
+  <si>
+    <t>Hold/UnHold button - Just added</t>
   </si>
 </sst>
 </file>
@@ -359,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -403,6 +406,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>